<commit_message>
Add download functionality for NO₂ measurements and locations data
</commit_message>
<xml_diff>
--- a/data/source/latest.xlsx
+++ b/data/source/latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icthva.sharepoint.com/sites/FDMCI_EDU_CMD_2526_Information_Design/Gedeelde documenten/Project KNMI - Air Pollution in Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F19D5A-4CFB-AC46-98E5-C0F79A49CDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{98F19D5A-4CFB-AC46-98E5-C0F79A49CDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD62817-946A-9044-9F4F-EEB2CF2A25C1}"/>
   <bookViews>
-    <workbookView xWindow="-1960" yWindow="-20980" windowWidth="38400" windowHeight="20980" xr2:uid="{061679CD-6275-624D-BE0D-931540F2E592}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="17280" xr2:uid="{061679CD-6275-624D-BE0D-931540F2E592}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="116">
   <si>
     <t>Tube ID</t>
   </si>
@@ -379,15 +379,22 @@
   </si>
   <si>
     <t>end of a quiet road on Campus, surrounded by a forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tube not covered from site but place in a zip lock container  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tube and Holder missing </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="d\-mm\-yy\ h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -431,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -441,9 +448,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -775,26 +786,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4782FC-93F9-CC4F-907E-65E1E4FF77E4}">
-  <dimension ref="A1:L81"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="7"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>2</v>
@@ -805,7 +817,7 @@
       <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -814,10 +826,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1">
         <v>45778</v>
@@ -828,7 +840,7 @@
       <c r="E2" s="3">
         <v>45807.314583333333</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7">
         <v>8.74</v>
       </c>
       <c r="K2" s="3"/>
@@ -836,10 +848,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>45778</v>
@@ -850,7 +862,7 @@
       <c r="E3" s="3">
         <v>45807.330555555556</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7">
         <v>43.04</v>
       </c>
       <c r="K3" s="3"/>
@@ -858,10 +870,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>45778</v>
@@ -872,7 +884,7 @@
       <c r="E4" s="3">
         <v>45807.356944444444</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7">
         <v>31.61</v>
       </c>
       <c r="K4" s="3"/>
@@ -880,10 +892,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
       <c r="C5" s="1">
         <v>45778</v>
@@ -894,7 +906,7 @@
       <c r="E5" s="3">
         <v>45807.339583333334</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7">
         <v>40.090000000000003</v>
       </c>
       <c r="K5" s="3"/>
@@ -902,10 +914,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>45778</v>
@@ -916,7 +928,7 @@
       <c r="E6" s="3">
         <v>45807.331944444442</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7">
         <v>33.51</v>
       </c>
       <c r="K6" s="3"/>
@@ -924,10 +936,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>45778</v>
@@ -938,7 +950,7 @@
       <c r="E7" s="3">
         <v>45807.320833333331</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="7">
         <v>49.31</v>
       </c>
       <c r="K7" s="3"/>
@@ -946,10 +958,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>45778</v>
@@ -960,7 +972,7 @@
       <c r="E8" s="3">
         <v>45807.392361111109</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="7">
         <v>50.49</v>
       </c>
       <c r="K8" s="3"/>
@@ -968,10 +980,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>45778</v>
@@ -982,7 +994,7 @@
       <c r="E9" s="3">
         <v>45807.401388888888</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>42.17</v>
       </c>
       <c r="K9" s="3"/>
@@ -990,10 +1002,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>45778</v>
@@ -1004,7 +1016,7 @@
       <c r="E10" s="3">
         <v>45807.408333333333</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <v>43.68</v>
       </c>
       <c r="K10" s="3"/>
@@ -1012,10 +1024,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="1">
         <v>45778</v>
@@ -1026,7 +1038,7 @@
       <c r="E11" s="3">
         <v>45807.417361111111</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>36.93</v>
       </c>
       <c r="K11" s="3"/>
@@ -1034,10 +1046,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
       </c>
       <c r="C12" s="1">
         <v>45778</v>
@@ -1048,7 +1060,7 @@
       <c r="E12" s="3">
         <v>45807.354861111111</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>43.11</v>
       </c>
       <c r="K12" s="3"/>
@@ -1056,10 +1068,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
       </c>
       <c r="C13" s="1">
         <v>45778</v>
@@ -1070,7 +1082,7 @@
       <c r="E13" s="3">
         <v>45807.348611111112</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>62.95</v>
       </c>
       <c r="K13" s="3"/>
@@ -1078,10 +1090,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>45778</v>
@@ -1092,7 +1104,7 @@
       <c r="E14" s="3">
         <v>45807.368055555555</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>71.2</v>
       </c>
       <c r="K14" s="3"/>
@@ -1100,10 +1112,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
         <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
       </c>
       <c r="C15" s="1">
         <v>45778</v>
@@ -1122,10 +1134,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
       </c>
       <c r="C16" s="1">
         <v>45778</v>
@@ -1136,7 +1148,7 @@
       <c r="E16" s="3">
         <v>45807.396527777775</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="7">
         <v>27.98</v>
       </c>
       <c r="K16" s="3"/>
@@ -1144,10 +1156,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
       </c>
       <c r="C17" s="1">
         <v>45778</v>
@@ -1158,7 +1170,7 @@
       <c r="E17" s="3">
         <v>45807.430555555555</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="7">
         <v>57.25</v>
       </c>
       <c r="K17" s="3"/>
@@ -1166,10 +1178,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
       </c>
       <c r="C18" s="1">
         <v>45778</v>
@@ -1180,7 +1192,7 @@
       <c r="E18" s="3">
         <v>45807.444444444445</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="7">
         <v>53.18</v>
       </c>
       <c r="K18" s="3"/>
@@ -1188,10 +1200,10 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
       </c>
       <c r="C19" s="1">
         <v>45778</v>
@@ -1202,7 +1214,7 @@
       <c r="E19" s="3">
         <v>45807.370138888888</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>82.12</v>
       </c>
       <c r="K19" s="3"/>
@@ -1210,10 +1222,10 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
       </c>
       <c r="C20" s="1">
         <v>45778</v>
@@ -1224,7 +1236,7 @@
       <c r="E20" s="3">
         <v>45807.349305555559</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="7">
         <v>27.08</v>
       </c>
       <c r="K20" s="3"/>
@@ -1232,10 +1244,10 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
       </c>
       <c r="C21" s="1">
         <v>45778</v>
@@ -1246,7 +1258,7 @@
       <c r="E21" s="3">
         <v>45807.295138888891</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="7">
         <v>9.14</v>
       </c>
       <c r="K21" s="3"/>
@@ -1254,1209 +1266,2418 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
       <c r="C22" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D22" s="3">
-        <v>45869.308333333334</v>
+        <v>45807.314583333333</v>
       </c>
       <c r="E22" s="3">
-        <v>45898.328472222223</v>
-      </c>
-      <c r="F22" s="2">
-        <v>14.643721192231496</v>
-      </c>
-      <c r="G22" s="2"/>
+        <v>45835.320833333331</v>
+      </c>
+      <c r="F22" s="7">
+        <v>11.381082971927803</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
       <c r="C23" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D23" s="3">
-        <v>45869.317361111112</v>
+        <v>45807.330555555556</v>
       </c>
       <c r="E23" s="3">
-        <v>45898.337500000001</v>
-      </c>
-      <c r="F23" s="2">
-        <v>43.185418515978988</v>
+        <v>45835.337500000001</v>
+      </c>
+      <c r="F23" s="7">
+        <v>42.581227381949532</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D24" s="3">
-        <v>45869.30972222222</v>
+        <v>45807.356944444444</v>
       </c>
       <c r="E24" s="3">
-        <v>45898.3125</v>
-      </c>
-      <c r="F24" s="2">
-        <v>11.125036386550901</v>
-      </c>
-      <c r="H24" s="2"/>
+        <v>45835.370833333334</v>
+      </c>
+      <c r="F24" s="7">
+        <v>19.969515134132852</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="C25" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D25" s="3">
-        <v>45869.330555555556</v>
+        <v>45807.339583333334</v>
       </c>
       <c r="E25" s="3">
-        <v>45898.351388888892</v>
-      </c>
-      <c r="F25" s="2">
-        <v>22.507403236143453</v>
+        <v>45835.35</v>
+      </c>
+      <c r="F25" s="7">
+        <v>13.701714475612988</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D26" s="3">
-        <v>45869.336111111108</v>
+        <v>45807.331944444442</v>
       </c>
       <c r="E26" s="3">
-        <v>45898.35833333333</v>
-      </c>
-      <c r="F26" s="2">
-        <v>27.997327373105819</v>
+        <v>45835.345138888886</v>
+      </c>
+      <c r="F26" s="7">
+        <v>4.6441884131461686</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D27" s="3">
-        <v>45869.352777777778</v>
+        <v>45807.320833333331</v>
       </c>
       <c r="E27" s="3">
-        <v>45898.374305555553</v>
-      </c>
-      <c r="F27" s="2">
-        <v>65.351257643385466</v>
+        <v>45835.332638888889</v>
+      </c>
+      <c r="F27" s="7">
+        <v>36.61350061407623</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
       <c r="C28" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D28" s="3">
-        <v>45869.365277777775</v>
+        <v>45807.392361111109</v>
       </c>
       <c r="E28" s="3">
-        <v>45898.383333333331</v>
-      </c>
-      <c r="F28" s="2">
-        <v>38.239128270501446</v>
+        <v>45835.402777777781</v>
+      </c>
+      <c r="F28" s="7">
+        <v>45.827203217857516</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
         <v>21</v>
       </c>
-      <c r="B29" t="s">
-        <v>22</v>
-      </c>
       <c r="C29" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D29" s="3">
-        <v>45869.378472222219</v>
+        <v>45807.401388888888</v>
       </c>
       <c r="E29" s="3">
-        <v>45898.392361111109</v>
-      </c>
-      <c r="F29" s="2">
-        <v>61.842363880328143</v>
+        <v>45835.418749999997</v>
+      </c>
+      <c r="F29" s="7">
+        <v>56.108931048244138</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
       <c r="C30" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D30" s="3">
-        <v>45869.397222222222</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2"/>
-      <c r="G30" t="s">
-        <v>48</v>
+        <v>45807.408333333333</v>
+      </c>
+      <c r="E30" s="3">
+        <v>45835.425000000003</v>
+      </c>
+      <c r="F30" s="7">
+        <v>43.959534880855358</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
       <c r="C31" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D31" s="3">
-        <v>45869.407638888886</v>
+        <v>45807.417361111111</v>
       </c>
       <c r="E31" s="3">
-        <v>45898.413194444445</v>
-      </c>
-      <c r="F31" s="2">
-        <v>31.26921109194258</v>
+        <v>45835.4375</v>
+      </c>
+      <c r="F31" s="7">
+        <v>15.863711145905752</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C32" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D32" s="3">
-        <v>45869.398611111108</v>
+        <v>45807.354861111111</v>
       </c>
       <c r="E32" s="3">
-        <v>45898.396527777775</v>
-      </c>
-      <c r="F32" s="2">
-        <v>45.593156748862718</v>
+        <v>45835.369444444441</v>
+      </c>
+      <c r="F32" s="7">
+        <v>29.798731568875283</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C33" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D33" s="3">
-        <v>45869.395138888889</v>
+        <v>45807.348611111112</v>
       </c>
       <c r="E33" s="3">
-        <v>45898.392361111109</v>
-      </c>
-      <c r="F33" s="2">
-        <v>27.410828053596418</v>
+        <v>45835.35833333333</v>
+      </c>
+      <c r="F33" s="7">
+        <v>31.661808815868127</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D34" s="3">
-        <v>45869.48333333333</v>
+        <v>45807.368055555555</v>
       </c>
       <c r="E34" s="3">
-        <v>45898.388194444444</v>
-      </c>
-      <c r="F34" s="2">
-        <v>29.268115196715719</v>
+        <v>45835.383333333331</v>
+      </c>
+      <c r="F34" s="7">
+        <v>49.689120654841105</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
       <c r="C35" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D35" s="3">
-        <v>45869.470833333333</v>
+        <v>45807.382638888892</v>
       </c>
       <c r="E35" s="3">
-        <v>45898.380555555559</v>
-      </c>
-      <c r="F35" s="2">
-        <v>47.705811324672148</v>
+        <v>45835.411111111112</v>
+      </c>
+      <c r="F35" s="7">
+        <v>49.356285631288927</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C36" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D36" s="3">
-        <v>45869.365277777775</v>
+        <v>45807.396527777775</v>
       </c>
       <c r="E36" s="3">
-        <v>45898.366666666669</v>
-      </c>
-      <c r="F36" s="2">
-        <v>70.348873344836591</v>
+        <v>45835.455555555556</v>
+      </c>
+      <c r="F36" s="7">
+        <v>25.810419534253622</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D37" s="3">
-        <v>45869.356249999997</v>
-      </c>
-      <c r="E37" s="3">
-        <v>45898.34652777778</v>
-      </c>
-      <c r="F37" s="2">
-        <v>40.175983507626285</v>
+        <v>45807.430555555555</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="7">
+        <v>-1.4200594911813723E-4</v>
+      </c>
+      <c r="G37" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D38" s="3">
-        <v>45869.35</v>
+        <v>45807.444444444445</v>
       </c>
       <c r="E38" s="3">
-        <v>45898.34097222222</v>
-      </c>
-      <c r="F38" s="2">
-        <v>28.298959147231443</v>
+        <v>45835.462500000001</v>
+      </c>
+      <c r="F38" s="7">
+        <v>44.576473440236676</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="C39" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D39" s="3">
-        <v>45869.446527777778</v>
+        <v>45807.370138888888</v>
       </c>
       <c r="E39" s="3">
-        <v>45898.326388888891</v>
-      </c>
-      <c r="F39" s="2">
-        <v>40.874583196547654</v>
+        <v>45835.386111111111</v>
+      </c>
+      <c r="F39" s="7">
+        <v>74.454438016827183</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C40" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D40" s="3">
-        <v>45869.338194444441</v>
+        <v>45807.349305555559</v>
       </c>
       <c r="E40" s="3">
-        <v>45898.333333333336</v>
-      </c>
-      <c r="F40" s="2">
-        <v>46.479619612373916</v>
+        <v>45835.361111111109</v>
+      </c>
+      <c r="F40" s="7">
+        <v>19.738779400828466</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="C41" s="1">
-        <v>45870</v>
+        <v>45809</v>
       </c>
       <c r="D41" s="3">
-        <v>45869.342361111114</v>
+        <v>45807.295138888891</v>
       </c>
       <c r="E41" s="3">
-        <v>45898.335416666669</v>
-      </c>
-      <c r="F41" s="2">
-        <v>29.111225708919516</v>
-      </c>
-      <c r="G41" t="s">
-        <v>49</v>
+        <v>45835.313194444447</v>
+      </c>
+      <c r="F41" s="7">
+        <v>7.6615813725406765</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
         <v>7</v>
       </c>
-      <c r="B42" t="s">
-        <v>8</v>
-      </c>
       <c r="C42" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D42" s="3">
-        <v>45898.32916666667</v>
+        <v>45835.325694444444</v>
       </c>
       <c r="E42" s="3">
-        <v>45931.321527777778</v>
-      </c>
-      <c r="F42" s="2">
-        <v>14.538449116808652</v>
+        <v>45869.306250000001</v>
+      </c>
+      <c r="F42" s="7">
+        <v>14.995672073358659</v>
+      </c>
+      <c r="G42" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
         <v>9</v>
       </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
       <c r="C43" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D43" s="3">
-        <v>45898.337500000001</v>
+        <v>45835.340277777781</v>
       </c>
       <c r="E43" s="3">
-        <v>45931.329861111109</v>
-      </c>
-      <c r="F43" s="2">
-        <v>49.92809499325076</v>
+        <v>45869.31527777778</v>
+      </c>
+      <c r="F43" s="7">
+        <v>48.519572569342039</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="C44" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D44" s="3">
-        <v>45898.3125</v>
+        <v>45835.373611111114</v>
       </c>
       <c r="E44" s="3">
-        <v>45931.319444444445</v>
-      </c>
-      <c r="F44" s="2">
-        <v>14.404551739660834</v>
+        <v>45869.335416666669</v>
+      </c>
+      <c r="F44" s="7">
+        <v>32.316202252439446</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D45" s="3">
-        <v>45898.351388888892</v>
+        <v>45835.35</v>
       </c>
       <c r="E45" s="3">
-        <v>45931.337500000001</v>
-      </c>
-      <c r="F45" s="2">
-        <v>23.151127055385661</v>
+        <v>45869.342361111114</v>
+      </c>
+      <c r="F45" s="7">
+        <v>23.830994166822251</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C46" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D46" s="3">
-        <v>45898.35833333333</v>
+        <v>45835.345138888886</v>
       </c>
       <c r="E46" s="3">
-        <v>45931.344444444447</v>
-      </c>
-      <c r="F46" s="2">
-        <v>30.294174521503486</v>
+        <v>45869.338194444441</v>
+      </c>
+      <c r="F46" s="7">
+        <v>39.205028176921601</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C47" s="1">
-        <v>45901</v>
+        <v>45839</v>
       </c>
       <c r="D47" s="3">
-        <v>45898.375</v>
-      </c>
-      <c r="E47" s="3">
-        <v>45931.365277777775</v>
-      </c>
-      <c r="F47" s="2">
-        <v>74.992525654226839</v>
+        <v>45835.332638888889</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
         <v>19</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45835.407638888886</v>
+      </c>
+      <c r="E48" s="3">
+        <v>45869.363888888889</v>
+      </c>
+      <c r="F48" s="7">
+        <v>40.530121730217772</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45835.422222222223</v>
+      </c>
+      <c r="E49" s="3">
+        <v>45869.377083333333</v>
+      </c>
+      <c r="F49" s="7">
+        <v>51.113652405097262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45835.429861111108</v>
+      </c>
+      <c r="E50" s="3">
+        <v>45869.395833333336</v>
+      </c>
+      <c r="F50" s="7">
+        <v>51.930382445364756</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45835.444444444445</v>
+      </c>
+      <c r="E51" s="3">
+        <v>45869.40625</v>
+      </c>
+      <c r="F51" s="7">
+        <v>30.841454927427325</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>28</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45835.369444444441</v>
+      </c>
+      <c r="E52" s="3">
+        <v>45869.356249999997</v>
+      </c>
+      <c r="F52" s="7">
+        <v>37.546358398544392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45835.359722222223</v>
+      </c>
+      <c r="E53" s="3">
+        <v>45869.35</v>
+      </c>
+      <c r="F53" s="7">
+        <v>48.113369805251892</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45835.384027777778</v>
+      </c>
+      <c r="E54" s="3">
+        <v>45869.365277777775</v>
+      </c>
+      <c r="F54" s="7">
+        <v>71.260028075523806</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45835.411111111112</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="7">
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>37</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D56" s="3">
+        <v>45835.455555555556</v>
+      </c>
+      <c r="E56" s="3">
+        <v>45869.395138888889</v>
+      </c>
+      <c r="F56" s="7">
+        <v>21.301595308395601</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D57" s="3">
+        <v>45835.436111111114</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D58" s="3">
+        <v>45835.462500000001</v>
+      </c>
+      <c r="E58" s="3">
+        <v>45869.398611111108</v>
+      </c>
+      <c r="F58" s="7">
+        <v>47.227645366113144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D59" s="3">
+        <v>45835.388194444444</v>
+      </c>
+      <c r="E59" s="3">
+        <v>45869.350694444445</v>
+      </c>
+      <c r="F59" s="7">
+        <v>72.325259481557381</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D60" s="3">
+        <v>45835.364583333336</v>
+      </c>
+      <c r="E60" s="3">
+        <v>45869.329861111109</v>
+      </c>
+      <c r="F60" s="7">
+        <v>25.196367370753485</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="1">
+        <v>45839</v>
+      </c>
+      <c r="D61" s="3">
+        <v>45835.313888888886</v>
+      </c>
+      <c r="E61" s="3">
+        <v>45869.30972222222</v>
+      </c>
+      <c r="F61" s="7">
+        <v>10.697229958792025</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D62" s="3">
+        <v>45869.308333333334</v>
+      </c>
+      <c r="E62" s="3">
+        <v>45898.328472222223</v>
+      </c>
+      <c r="F62" s="7">
+        <v>14.643721192231496</v>
+      </c>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D63" s="3">
+        <v>45869.317361111112</v>
+      </c>
+      <c r="E63" s="3">
+        <v>45898.337500000001</v>
+      </c>
+      <c r="F63" s="7">
+        <v>43.185418515978988</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D64" s="3">
+        <v>45869.336111111108</v>
+      </c>
+      <c r="E64" s="3">
+        <v>45898.35833333333</v>
+      </c>
+      <c r="F64" s="7">
+        <v>27.997327373105819</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D65" s="3">
+        <v>45869.342361111114</v>
+      </c>
+      <c r="E65" s="3">
+        <v>45898.335416666669</v>
+      </c>
+      <c r="F65" s="7">
+        <v>29.111225708919516</v>
+      </c>
+      <c r="G65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D66" s="3">
+        <v>45869.338194444441</v>
+      </c>
+      <c r="E66" s="3">
+        <v>45898.333333333336</v>
+      </c>
+      <c r="F66" s="7">
+        <v>46.479619612373916</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D67" s="3">
+        <v>45869.446527777778</v>
+      </c>
+      <c r="E67" s="3">
+        <v>45898.326388888891</v>
+      </c>
+      <c r="F67" s="7">
+        <v>40.874583196547654</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="1">
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D68" s="3">
+        <v>45869.365277777775</v>
+      </c>
+      <c r="E68" s="3">
+        <v>45898.383333333331</v>
+      </c>
+      <c r="F68" s="7">
+        <v>38.239128270501446</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D69" s="3">
+        <v>45869.378472222219</v>
+      </c>
+      <c r="E69" s="3">
+        <v>45898.392361111109</v>
+      </c>
+      <c r="F69" s="7">
+        <v>61.842363880328143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D70" s="3">
+        <v>45869.397222222222</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="G70" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>26</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D71" s="3">
+        <v>45869.407638888886</v>
+      </c>
+      <c r="E71" s="3">
+        <v>45898.413194444445</v>
+      </c>
+      <c r="F71" s="7">
+        <v>31.26921109194258</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D72" s="3">
+        <v>45869.356249999997</v>
+      </c>
+      <c r="E72" s="3">
+        <v>45898.34652777778</v>
+      </c>
+      <c r="F72" s="7">
+        <v>40.175983507626285</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C73" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D73" s="3">
+        <v>45869.35</v>
+      </c>
+      <c r="E73" s="3">
+        <v>45898.34097222222</v>
+      </c>
+      <c r="F73" s="7">
+        <v>28.298959147231443</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D74" s="3">
+        <v>45869.365277777775</v>
+      </c>
+      <c r="E74" s="3">
+        <v>45898.366666666669</v>
+      </c>
+      <c r="F74" s="7">
+        <v>70.348873344836591</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C75" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D75" s="3">
+        <v>45869.470833333333</v>
+      </c>
+      <c r="E75" s="3">
+        <v>45898.380555555559</v>
+      </c>
+      <c r="F75" s="7">
+        <v>47.705811324672148</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>37</v>
+      </c>
+      <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D76" s="3">
+        <v>45869.395138888889</v>
+      </c>
+      <c r="E76" s="3">
+        <v>45898.392361111109</v>
+      </c>
+      <c r="F76" s="7">
+        <v>27.410828053596418</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>39</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D77" s="3">
+        <v>45869.48333333333</v>
+      </c>
+      <c r="E77" s="3">
+        <v>45898.388194444444</v>
+      </c>
+      <c r="F77" s="7">
+        <v>29.268115196715719</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>41</v>
+      </c>
+      <c r="B78" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D78" s="3">
+        <v>45869.398611111108</v>
+      </c>
+      <c r="E78" s="3">
+        <v>45898.396527777775</v>
+      </c>
+      <c r="F78" s="7">
+        <v>45.593156748862718</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B79" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D79" s="3">
+        <v>45869.352777777778</v>
+      </c>
+      <c r="E79" s="3">
+        <v>45898.374305555553</v>
+      </c>
+      <c r="F79" s="7">
+        <v>65.351257643385466</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D80" s="3">
+        <v>45869.330555555556</v>
+      </c>
+      <c r="E80" s="3">
+        <v>45898.351388888892</v>
+      </c>
+      <c r="F80" s="7">
+        <v>22.507403236143453</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>47</v>
+      </c>
+      <c r="B81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C81" s="1">
+        <v>45870</v>
+      </c>
+      <c r="D81" s="3">
+        <v>45869.30972222222</v>
+      </c>
+      <c r="E81" s="3">
+        <v>45898.3125</v>
+      </c>
+      <c r="F81" s="7">
+        <v>11.125036386550901</v>
+      </c>
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1">
         <v>45901</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D82" s="3">
+        <v>45898.32916666667</v>
+      </c>
+      <c r="E82" s="3">
+        <v>45931.321527777778</v>
+      </c>
+      <c r="F82" s="7">
+        <v>14.538449116808652</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D83" s="3">
+        <v>45898.337500000001</v>
+      </c>
+      <c r="E83" s="3">
+        <v>45931.329861111109</v>
+      </c>
+      <c r="F83" s="7">
+        <v>49.92809499325076</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D84" s="3">
+        <v>45898.35833333333</v>
+      </c>
+      <c r="E84" s="3">
+        <v>45931.344444444447</v>
+      </c>
+      <c r="F84" s="7">
+        <v>30.294174521503486</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D85" s="3">
+        <v>45898.335416666669</v>
+      </c>
+      <c r="E85" s="3">
+        <v>45931.356249999997</v>
+      </c>
+      <c r="F85" s="7">
+        <v>36.059942753262739</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D86" s="3">
+        <v>45898.333333333336</v>
+      </c>
+      <c r="E86" s="3">
+        <v>45931.354166666664</v>
+      </c>
+      <c r="F86" s="7">
+        <v>54.153624276101283</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>18</v>
+      </c>
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D87" s="3">
+        <v>45898.3125</v>
+      </c>
+      <c r="E87" s="3">
+        <v>45931.34375</v>
+      </c>
+      <c r="F87" s="7">
+        <v>41.844365942670457</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D88" s="3">
         <v>45898.383333333331</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E88" s="3">
         <v>45931.377083333333</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F88" s="7">
         <v>47.120445731291554</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" t="s">
         <v>21</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C89" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D89" s="3">
+        <v>45898.393055555556</v>
+      </c>
+      <c r="E89" s="3">
+        <v>45931.384722222225</v>
+      </c>
+      <c r="F89" s="7">
+        <v>58.410086431128072</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D90" s="3">
+        <v>45898.40347222222</v>
+      </c>
+      <c r="E90" s="3">
+        <v>45931.307638888888</v>
+      </c>
+      <c r="F90" s="7">
+        <v>56.775203611285534</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91" t="s">
+        <v>25</v>
+      </c>
+      <c r="C91" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D91" s="3">
+        <v>45898.413194444445</v>
+      </c>
+      <c r="E91" s="3">
+        <v>45931.4</v>
+      </c>
+      <c r="F91" s="7">
+        <v>39.859916793209727</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D92" s="3">
+        <v>45898.34652777778</v>
+      </c>
+      <c r="E92" s="3">
+        <v>45931.376388888886</v>
+      </c>
+      <c r="F92" s="7">
+        <v>45.731382180363333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>30</v>
+      </c>
+      <c r="B93" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D93" s="3">
+        <v>45898.34097222222</v>
+      </c>
+      <c r="E93" s="3">
+        <v>45931.365277777775</v>
+      </c>
+      <c r="F93" s="7">
+        <v>45.611668504680374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D94" s="3">
+        <v>45898.366666666669</v>
+      </c>
+      <c r="E94" s="3">
+        <v>45931.388888888891</v>
+      </c>
+      <c r="F94" s="7">
+        <v>68.16698927072386</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>34</v>
+      </c>
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D95" s="3">
+        <v>45898.380555555559</v>
+      </c>
+      <c r="E95" s="3">
+        <v>45931.411805555559</v>
+      </c>
+      <c r="F95" s="7">
+        <v>49.678242671663554</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D96" s="3">
+        <v>45898.392361111109</v>
+      </c>
+      <c r="E96" s="3">
+        <v>45931.428472222222</v>
+      </c>
+      <c r="F96" s="7">
+        <v>36.106947266658437</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D97" s="3">
+        <v>45898.388194444444</v>
+      </c>
+      <c r="E97" s="3">
+        <v>45931.42291666667</v>
+      </c>
+      <c r="F97" s="7">
+        <v>32.669563862795997</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D98" s="3">
+        <v>45898.396527777775</v>
+      </c>
+      <c r="E98" s="3">
+        <v>45931.429861111108</v>
+      </c>
+      <c r="F98" s="7">
+        <v>51.203574493973555</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>43</v>
+      </c>
+      <c r="B99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C99" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D99" s="3">
+        <v>45898.375</v>
+      </c>
+      <c r="E99" s="3">
+        <v>45931.365277777775</v>
+      </c>
+      <c r="F99" s="7">
+        <v>74.992525654226839</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>45</v>
+      </c>
+      <c r="B100" t="s">
+        <v>44</v>
+      </c>
+      <c r="C100" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D100" s="3">
+        <v>45898.351388888892</v>
+      </c>
+      <c r="E100" s="3">
+        <v>45931.337500000001</v>
+      </c>
+      <c r="F100" s="7">
+        <v>23.151127055385661</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>47</v>
+      </c>
+      <c r="B101" t="s">
+        <v>46</v>
+      </c>
+      <c r="C101" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D101" s="3">
+        <v>45898.3125</v>
+      </c>
+      <c r="E101" s="3">
+        <v>45931.319444444445</v>
+      </c>
+      <c r="F101" s="7">
+        <v>14.404551739660834</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D102" s="3">
+        <v>45931.320833333331</v>
+      </c>
+      <c r="E102" s="3">
+        <v>45960.343055555553</v>
+      </c>
+      <c r="F102" s="7">
+        <v>12.540419678936304</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>10</v>
+      </c>
+      <c r="B103" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D103" s="3">
+        <v>45931.329861111109</v>
+      </c>
+      <c r="E103" s="3">
+        <v>45960.352083333331</v>
+      </c>
+      <c r="F103" s="7">
+        <v>34.866715985944289</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D104" s="3">
+        <v>45931.34375</v>
+      </c>
+      <c r="E104" s="3">
+        <v>45960.365277777775</v>
+      </c>
+      <c r="F104" s="7">
+        <v>26.09629544098992</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>14</v>
+      </c>
+      <c r="B105" t="s">
+        <v>13</v>
+      </c>
+      <c r="C105" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D105" s="3">
+        <v>45931.356249999997</v>
+      </c>
+      <c r="E105" s="3">
+        <v>45960.370138888888</v>
+      </c>
+      <c r="F105" s="7">
+        <v>24.870516660787221</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>16</v>
+      </c>
+      <c r="B106" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D106" s="3">
+        <v>45931.354166666664</v>
+      </c>
+      <c r="E106" s="3">
+        <v>45960.367361111108</v>
+      </c>
+      <c r="F106" s="7">
+        <v>27.481491044907841</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D107" s="3">
+        <v>45931.34375</v>
+      </c>
+      <c r="E107" s="3">
+        <v>45960.36041666667</v>
+      </c>
+      <c r="F107" s="7">
+        <v>34.29337676783441</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>20</v>
+      </c>
+      <c r="B108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D108" s="3">
+        <v>45931.376388888886</v>
+      </c>
+      <c r="E108" s="3">
+        <v>45960.349305555559</v>
+      </c>
+      <c r="F108" s="7">
+        <v>35.724776166868068</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D49" s="3">
-        <v>45898.393055555556</v>
-      </c>
-      <c r="E49" s="3">
-        <v>45931.384722222225</v>
-      </c>
-      <c r="F49" s="2">
-        <v>58.410086431128072</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B109" t="s">
+        <v>21</v>
+      </c>
+      <c r="C109" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D109" s="3">
+        <v>45931.383333333331</v>
+      </c>
+      <c r="E109" s="3">
+        <v>45960.400694444441</v>
+      </c>
+      <c r="F109" s="7">
+        <v>32.625053331768974</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
         <v>23</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C110" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D110" s="3">
+        <v>45931.390277777777</v>
+      </c>
+      <c r="E110" s="3">
+        <v>45960.407638888886</v>
+      </c>
+      <c r="F110" s="7">
+        <v>35.670058309400751</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" t="s">
+        <v>25</v>
+      </c>
+      <c r="C111" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D111" s="3">
+        <v>45931.4</v>
+      </c>
+      <c r="E111" s="3">
+        <v>45960.416666666664</v>
+      </c>
+      <c r="F111" s="7">
+        <v>23.345596869440698</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>28</v>
+      </c>
+      <c r="B112" t="s">
+        <v>27</v>
+      </c>
+      <c r="C112" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D112" s="3">
+        <v>45931.376388888886</v>
+      </c>
+      <c r="E112" s="3">
+        <v>45960.387499999997</v>
+      </c>
+      <c r="F112" s="7">
+        <v>28.861263547396888</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>30</v>
+      </c>
+      <c r="B113" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D113" s="3">
+        <v>45931.366666666669</v>
+      </c>
+      <c r="E113" s="3">
+        <v>45960.379166666666</v>
+      </c>
+      <c r="F113" s="7">
+        <v>41.652999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>32</v>
+      </c>
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
+      <c r="C114" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D114" s="3">
+        <v>45931.388888888891</v>
+      </c>
+      <c r="E114" s="3">
+        <v>45960.397222222222</v>
+      </c>
+      <c r="F114" s="7">
+        <v>62.151938056436556</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>34</v>
+      </c>
+      <c r="B115" t="s">
+        <v>33</v>
+      </c>
+      <c r="C115" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D115" s="3">
+        <v>45931.411805555559</v>
+      </c>
+      <c r="E115" s="3">
+        <v>45960.415277777778</v>
+      </c>
+      <c r="F115" s="7">
+        <v>36.267418318582614</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>37</v>
+      </c>
+      <c r="B116" t="s">
+        <v>36</v>
+      </c>
+      <c r="C116" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D116" s="3">
+        <v>45931.428472222222</v>
+      </c>
+      <c r="E116" s="3">
+        <v>45960.431944444441</v>
+      </c>
+      <c r="F116" s="7">
+        <v>29.739283021237746</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>39</v>
+      </c>
+      <c r="B117" t="s">
+        <v>38</v>
+      </c>
+      <c r="C117" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D117" s="3">
+        <v>45931.42291666667</v>
+      </c>
+      <c r="E117" s="3">
+        <v>45960.424305555556</v>
+      </c>
+      <c r="F117" s="7">
+        <v>8.0519452418173998</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>41</v>
+      </c>
+      <c r="B118" t="s">
+        <v>40</v>
+      </c>
+      <c r="C118" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D118" s="3">
+        <v>45931.429861111108</v>
+      </c>
+      <c r="E118" s="3">
+        <v>45960.438888888886</v>
+      </c>
+      <c r="F118" s="7">
+        <v>41.046855095812418</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>43</v>
+      </c>
+      <c r="B119" t="s">
+        <v>42</v>
+      </c>
+      <c r="C119" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D119" s="3">
+        <v>45931.364583333336</v>
+      </c>
+      <c r="E119" s="3">
+        <v>45960.381249999999</v>
+      </c>
+      <c r="F119" s="7">
+        <v>63.004110806037168</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>45</v>
+      </c>
+      <c r="B120" t="s">
+        <v>44</v>
+      </c>
+      <c r="C120" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D120" s="3">
+        <v>45931.336805555555</v>
+      </c>
+      <c r="E120" s="3">
+        <v>45960.359027777777</v>
+      </c>
+      <c r="F120" s="7">
+        <v>19.861705156234382</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>47</v>
+      </c>
+      <c r="B121" t="s">
+        <v>46</v>
+      </c>
+      <c r="C121" s="1">
+        <v>45931</v>
+      </c>
+      <c r="D121" s="3">
+        <v>45931.319444444445</v>
+      </c>
+      <c r="E121" s="3">
+        <v>45960.343055555553</v>
+      </c>
+      <c r="F121" s="7">
+        <v>9.640439324690341</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D122" s="3">
+        <v>45960.343055555553</v>
+      </c>
+      <c r="E122" s="3">
+        <v>45995.348611111112</v>
+      </c>
+      <c r="F122" s="7">
+        <v>22.029759956344304</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>10</v>
+      </c>
+      <c r="B123" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D123" s="3">
+        <v>45960.352083333331</v>
+      </c>
+      <c r="E123" s="3">
+        <v>45995.356944444444</v>
+      </c>
+      <c r="F123" s="7">
+        <v>44.896983747383786</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D124" s="3">
+        <v>45960.365277777775</v>
+      </c>
+      <c r="E124" s="3">
+        <v>45995.375</v>
+      </c>
+      <c r="F124" s="7">
+        <v>39.370024036666564</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>14</v>
+      </c>
+      <c r="B125" t="s">
+        <v>13</v>
+      </c>
+      <c r="C125" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D125" s="3">
+        <v>45960.370138888888</v>
+      </c>
+      <c r="E125" s="3">
+        <v>45995.376388888886</v>
+      </c>
+      <c r="F125" s="7">
+        <v>25.487090080355863</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>16</v>
+      </c>
+      <c r="B126" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D126" s="3">
+        <v>45960.40902777778</v>
+      </c>
+      <c r="E126" s="3">
+        <v>45995.371527777781</v>
+      </c>
+      <c r="F126" s="7">
+        <v>43.834577121528362</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C127" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D127" s="3">
+        <v>45960.402083333334</v>
+      </c>
+      <c r="E127" s="3">
+        <v>45995.359027777777</v>
+      </c>
+      <c r="F127" s="7">
+        <v>42.389466958731319</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>20</v>
+      </c>
+      <c r="B128" t="s">
+        <v>19</v>
+      </c>
+      <c r="C128" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D128" s="3">
+        <v>45960.390972222223</v>
+      </c>
+      <c r="E128" s="3">
+        <v>45995.407638888886</v>
+      </c>
+      <c r="F128" s="7">
+        <v>51.293539578765412</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>22</v>
+      </c>
+      <c r="B129" t="s">
+        <v>21</v>
+      </c>
+      <c r="C129" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D129" s="3">
+        <v>45960.399305555555</v>
+      </c>
+      <c r="E129" s="3">
+        <v>45995.357638888891</v>
+      </c>
+      <c r="F129" s="7">
+        <v>60.147091054256691</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D50" s="3">
-        <v>45898.40347222222</v>
-      </c>
-      <c r="E50" s="3">
-        <v>45931.307638888888</v>
-      </c>
-      <c r="F50" s="2">
-        <v>56.775203611285534</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B130" t="s">
+        <v>23</v>
+      </c>
+      <c r="C130" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D130" s="3">
+        <v>45960.40625</v>
+      </c>
+      <c r="E130" s="3">
+        <v>45995.417361111111</v>
+      </c>
+      <c r="F130" s="7">
+        <v>50.186424939017229</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" t="s">
         <v>25</v>
       </c>
-      <c r="B51" t="s">
-        <v>26</v>
-      </c>
-      <c r="C51" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D51" s="3">
-        <v>45898.413194444445</v>
-      </c>
-      <c r="E51" s="3">
-        <v>45931.4</v>
-      </c>
-      <c r="F51" s="2">
-        <v>39.859916793209727</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="C131" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D131" s="3">
+        <v>45960.416666666664</v>
+      </c>
+      <c r="E131" s="3">
+        <v>45995.432638888888</v>
+      </c>
+      <c r="F131" s="7">
+        <v>32.951177276633253</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>28</v>
+      </c>
+      <c r="B132" t="s">
+        <v>27</v>
+      </c>
+      <c r="C132" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D132" s="3">
+        <v>45960.387499999997</v>
+      </c>
+      <c r="E132" s="3">
+        <v>45995.394444444442</v>
+      </c>
+      <c r="F132" s="7">
+        <v>43.500078551121454</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>30</v>
+      </c>
+      <c r="B133" t="s">
+        <v>29</v>
+      </c>
+      <c r="C133" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D133" s="3">
+        <v>45960.379166666666</v>
+      </c>
+      <c r="E133" s="3">
+        <v>45995.387499999997</v>
+      </c>
+      <c r="F133" s="7">
+        <v>45.227133455382742</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>32</v>
+      </c>
+      <c r="B134" t="s">
+        <v>31</v>
+      </c>
+      <c r="C134" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D134" s="3">
+        <v>45960.397222222222</v>
+      </c>
+      <c r="E134" s="3">
+        <v>45995.405555555553</v>
+      </c>
+      <c r="F134" s="7">
+        <v>77.237459723434128</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>34</v>
+      </c>
+      <c r="B135" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D135" s="3">
+        <v>45960.415277777778</v>
+      </c>
+      <c r="E135" s="3">
+        <v>45995.42083333333</v>
+      </c>
+      <c r="F135" s="7">
+        <v>48.29815727138768</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>37</v>
+      </c>
+      <c r="B136" t="s">
+        <v>36</v>
+      </c>
+      <c r="C136" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D136" s="3">
+        <v>45960.431944444441</v>
+      </c>
+      <c r="E136" s="3">
+        <v>45995.443749999999</v>
+      </c>
+      <c r="F136" s="7">
+        <v>38.531257547833334</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>39</v>
+      </c>
+      <c r="B137" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D137" s="3">
+        <v>45960.424305555556</v>
+      </c>
+      <c r="E137" s="3">
+        <v>45995.435416666667</v>
+      </c>
+      <c r="F137" s="7">
+        <v>33.346091237258115</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>41</v>
+      </c>
+      <c r="B138" t="s">
         <v>40</v>
       </c>
-      <c r="B52" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D52" s="3">
-        <v>45898.396527777775</v>
-      </c>
-      <c r="E52" s="3">
-        <v>45931.429861111108</v>
-      </c>
-      <c r="F52" s="2">
-        <v>51.203574493973555</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D53" s="3">
-        <v>45898.392361111109</v>
-      </c>
-      <c r="E53" s="3">
-        <v>45931.428472222222</v>
-      </c>
-      <c r="F53" s="2">
-        <v>36.106947266658437</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>38</v>
-      </c>
-      <c r="B54" t="s">
-        <v>39</v>
-      </c>
-      <c r="C54" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D54" s="3">
-        <v>45898.388194444444</v>
-      </c>
-      <c r="E54" s="3">
-        <v>45931.42291666667</v>
-      </c>
-      <c r="F54" s="2">
-        <v>32.669563862795997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D55" s="3">
-        <v>45898.380555555559</v>
-      </c>
-      <c r="E55" s="3">
-        <v>45931.411805555559</v>
-      </c>
-      <c r="F55" s="2">
-        <v>49.678242671663554</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D56" s="3">
-        <v>45898.366666666669</v>
-      </c>
-      <c r="E56" s="3">
-        <v>45931.388888888891</v>
-      </c>
-      <c r="F56" s="2">
-        <v>68.16698927072386</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>27</v>
-      </c>
-      <c r="B57" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D57" s="3">
-        <v>45898.34652777778</v>
-      </c>
-      <c r="E57" s="3">
-        <v>45931.376388888886</v>
-      </c>
-      <c r="F57" s="2">
-        <v>45.731382180363333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>29</v>
-      </c>
-      <c r="B58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D58" s="3">
-        <v>45898.34097222222</v>
-      </c>
-      <c r="E58" s="3">
-        <v>45931.365277777775</v>
-      </c>
-      <c r="F58" s="2">
-        <v>45.611668504680374</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>17</v>
-      </c>
-      <c r="B59" t="s">
-        <v>18</v>
-      </c>
-      <c r="C59" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D59" s="3">
-        <v>45898.3125</v>
-      </c>
-      <c r="E59" s="3">
-        <v>45931.34375</v>
-      </c>
-      <c r="F59" s="2">
-        <v>41.844365942670457</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D60" s="3">
-        <v>45898.333333333336</v>
-      </c>
-      <c r="E60" s="3">
-        <v>45931.354166666664</v>
-      </c>
-      <c r="F60" s="2">
-        <v>54.153624276101283</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D61" s="3">
-        <v>45898.335416666669</v>
-      </c>
-      <c r="E61" s="3">
-        <v>45931.356249999997</v>
-      </c>
-      <c r="F61" s="2">
-        <v>36.059942753262739</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D62" s="3">
-        <v>45931.320833333331</v>
-      </c>
-      <c r="E62" s="3">
+      <c r="C138" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D138" s="3">
+        <v>45960.438888888886</v>
+      </c>
+      <c r="E138" s="3">
+        <v>45995.447916666664</v>
+      </c>
+      <c r="F138" s="7">
+        <v>55.766012728759506</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>43</v>
+      </c>
+      <c r="B139" t="s">
+        <v>42</v>
+      </c>
+      <c r="C139" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D139" s="3">
+        <v>45960.381249999999</v>
+      </c>
+      <c r="E139" s="3">
+        <v>45995.395833333336</v>
+      </c>
+      <c r="F139" s="7">
+        <v>84.806647459106088</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>45</v>
+      </c>
+      <c r="B140" t="s">
+        <v>44</v>
+      </c>
+      <c r="C140" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D140" s="3">
+        <v>45960.359027777777</v>
+      </c>
+      <c r="E140" s="3">
+        <v>45995.366666666669</v>
+      </c>
+      <c r="F140" s="7">
+        <v>30.44945094985864</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" t="s">
+        <v>46</v>
+      </c>
+      <c r="C141" s="1">
+        <v>45962</v>
+      </c>
+      <c r="D141" s="3">
         <v>45960.343055555553</v>
       </c>
-      <c r="F62" s="2">
-        <v>12.540419678936304</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" t="s">
-        <v>10</v>
-      </c>
-      <c r="C63" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D63" s="3">
-        <v>45931.329861111109</v>
-      </c>
-      <c r="E63" s="3">
-        <v>45960.352083333331</v>
-      </c>
-      <c r="F63" s="2">
-        <v>34.866715985944289</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>46</v>
-      </c>
-      <c r="B64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D64" s="3">
-        <v>45931.319444444445</v>
-      </c>
-      <c r="E64" s="3">
-        <v>45960.343055555553</v>
-      </c>
-      <c r="F64" s="2">
-        <v>9.640439324690341</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>44</v>
-      </c>
-      <c r="B65" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D65" s="3">
-        <v>45931.336805555555</v>
-      </c>
-      <c r="E65" s="3">
-        <v>45960.359027777777</v>
-      </c>
-      <c r="F65" s="2">
-        <v>19.861705156234382</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D66" s="3">
-        <v>45931.34375</v>
-      </c>
-      <c r="E66" s="3">
-        <v>45960.365277777775</v>
-      </c>
-      <c r="F66" s="2">
-        <v>26.09629544098992</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" t="s">
-        <v>43</v>
-      </c>
-      <c r="C67" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D67" s="3">
-        <v>45931.364583333336</v>
-      </c>
-      <c r="E67" s="3">
-        <v>45960.381249999999</v>
-      </c>
-      <c r="F67" s="2">
-        <v>63.004110806037168</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B68" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D68" s="3">
-        <v>45931.376388888886</v>
-      </c>
-      <c r="E68" s="3">
-        <v>45960.349305555559</v>
-      </c>
-      <c r="F68" s="2">
-        <v>35.724776166868068</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>21</v>
-      </c>
-      <c r="B69" t="s">
-        <v>22</v>
-      </c>
-      <c r="C69" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D69" s="3">
-        <v>45931.383333333331</v>
-      </c>
-      <c r="E69" s="3">
-        <v>45960.400694444441</v>
-      </c>
-      <c r="F69" s="2">
-        <v>32.625053331768974</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D70" s="3">
-        <v>45931.390277777777</v>
-      </c>
-      <c r="E70" s="3">
-        <v>45960.407638888886</v>
-      </c>
-      <c r="F70" s="2">
-        <v>35.670058309400751</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D71" s="3">
-        <v>45931.4</v>
-      </c>
-      <c r="E71" s="3">
-        <v>45960.416666666664</v>
-      </c>
-      <c r="F71" s="2">
-        <v>23.345596869440698</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>40</v>
-      </c>
-      <c r="B72" t="s">
-        <v>41</v>
-      </c>
-      <c r="C72" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D72" s="3">
-        <v>45931.429861111108</v>
-      </c>
-      <c r="E72" s="3">
-        <v>45960.438888888886</v>
-      </c>
-      <c r="F72" s="2">
-        <v>41.046855095812418</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>36</v>
-      </c>
-      <c r="B73" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D73" s="3">
-        <v>45931.428472222222</v>
-      </c>
-      <c r="E73" s="3">
-        <v>45960.431944444441</v>
-      </c>
-      <c r="F73" s="2">
-        <v>29.739283021237746</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>38</v>
-      </c>
-      <c r="B74" t="s">
-        <v>39</v>
-      </c>
-      <c r="C74" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D74" s="3">
-        <v>45931.42291666667</v>
-      </c>
-      <c r="E74" s="3">
-        <v>45960.424305555556</v>
-      </c>
-      <c r="F74" s="2">
-        <v>8.0519452418173998</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>33</v>
-      </c>
-      <c r="B75" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D75" s="3">
-        <v>45931.411805555559</v>
-      </c>
-      <c r="E75" s="3">
-        <v>45960.415277777778</v>
-      </c>
-      <c r="F75" s="2">
-        <v>36.267418318582614</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>31</v>
-      </c>
-      <c r="B76" t="s">
-        <v>32</v>
-      </c>
-      <c r="C76" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D76" s="3">
-        <v>45931.388888888891</v>
-      </c>
-      <c r="E76" s="3">
-        <v>45960.397222222222</v>
-      </c>
-      <c r="F76" s="2">
-        <v>62.151938056436556</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>27</v>
-      </c>
-      <c r="B77" t="s">
-        <v>28</v>
-      </c>
-      <c r="C77" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D77" s="3">
-        <v>45931.376388888886</v>
-      </c>
-      <c r="E77" s="3">
-        <v>45960.387499999997</v>
-      </c>
-      <c r="F77" s="2">
-        <v>28.861263547396888</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>29</v>
-      </c>
-      <c r="B78" t="s">
-        <v>30</v>
-      </c>
-      <c r="C78" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D78" s="3">
-        <v>45931.366666666669</v>
-      </c>
-      <c r="E78" s="3">
-        <v>45960.379166666666</v>
-      </c>
-      <c r="F78">
-        <v>41.652999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>17</v>
-      </c>
-      <c r="B79" t="s">
-        <v>18</v>
-      </c>
-      <c r="C79" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D79" s="3">
-        <v>45931.34375</v>
-      </c>
-      <c r="E79" s="3">
-        <v>45960.36041666667</v>
-      </c>
-      <c r="F79" s="2">
-        <v>34.29337676783441</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>15</v>
-      </c>
-      <c r="B80" t="s">
-        <v>16</v>
-      </c>
-      <c r="C80" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D80" s="3">
-        <v>45931.354166666664</v>
-      </c>
-      <c r="E80" s="3">
-        <v>45960.367361111108</v>
-      </c>
-      <c r="F80" s="2">
-        <v>27.481491044907841</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" t="s">
-        <v>14</v>
-      </c>
-      <c r="C81" s="1">
-        <v>45931</v>
-      </c>
-      <c r="D81" s="3">
-        <v>45931.356249999997</v>
-      </c>
-      <c r="E81" s="3">
-        <v>45960.370138888888</v>
-      </c>
-      <c r="F81" s="2">
-        <v>24.870516660787221</v>
+      <c r="E141" s="3">
+        <v>45995.329861111109</v>
+      </c>
+      <c r="F141" s="7">
+        <v>18.247068615157321</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L141">
+    <sortCondition ref="C2:C141"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2466,7 +3687,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2840,6 +4061,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d2effc7-4260-41d0-876f-94073c520d46">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007862564C6B7D034CBD34C383492C7D58" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="53b9cbb27ea0be9acc74f77401b342f9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d2effc7-4260-41d0-876f-94073c520d46" xmlns:ns3="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1083e288036101acb4c2841bf829040b" ns2:_="" ns3:_="">
     <xsd:import namespace="0d2effc7-4260-41d0-876f-94073c520d46"/>
@@ -3034,28 +4275,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A726DE-ED6C-4B29-9DAB-510946DBBF5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9"/>
+    <ds:schemaRef ds:uri="0d2effc7-4260-41d0-876f-94073c520d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d2effc7-4260-41d0-876f-94073c520d46">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D234CA42-CCAF-4C6D-881C-C8492E2A638A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E78832D-A6B5-48BB-AAD5-1903E204D7FF}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FC27487-92EB-4918-ABF3-A8DCA0ADCB9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -3071,29 +4317,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FFC9629-7490-42DA-B948-18448300B0CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{062558DA-3674-41B9-9A98-88E8CAE4C891}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="0d2effc7-4260-41d0-876f-94073c520d46"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: update Excel file path for importing data
</commit_message>
<xml_diff>
--- a/data/source/latest.xlsx
+++ b/data/source/latest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icthva.sharepoint.com/sites/FDMCI_EDU_CMD_2526_Information_Design/Gedeelde documenten/Project KNMI - Air Pollution in Africa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://knmi-my.sharepoint.com/personal/bas_mijling_knmi_nl/Documents/TubeSat Ghana/HvA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{98F19D5A-4CFB-AC46-98E5-C0F79A49CDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD62817-946A-9044-9F4F-EEB2CF2A25C1}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="13_ncr:1_{98F19D5A-4CFB-AC46-98E5-C0F79A49CDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F90BC828-CC78-F340-9B3B-367FBC68F4F5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="17280" xr2:uid="{061679CD-6275-624D-BE0D-931540F2E592}"/>
+    <workbookView xWindow="-10520" yWindow="-27360" windowWidth="34480" windowHeight="27360" xr2:uid="{061679CD-6275-624D-BE0D-931540F2E592}"/>
   </bookViews>
   <sheets>
     <sheet name="Measurements" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="116">
   <si>
     <t>Tube ID</t>
   </si>
@@ -438,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -452,9 +452,10 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,6 +468,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -786,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4782FC-93F9-CC4F-907E-65E1E4FF77E4}">
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3674,6 +3679,402 @@
         <v>18.247068615157321</v>
       </c>
     </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D142" s="3">
+        <v>45995.348611111112</v>
+      </c>
+      <c r="E142" s="3">
+        <v>46029.332638888889</v>
+      </c>
+      <c r="F142" s="7">
+        <v>14.32373502204136</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>10</v>
+      </c>
+      <c r="B143" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D143" s="3">
+        <v>45995.356944444444</v>
+      </c>
+      <c r="E143" s="3">
+        <v>46029.352083333331</v>
+      </c>
+      <c r="F143" s="7">
+        <v>43.938708195479563</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>47</v>
+      </c>
+      <c r="B144" t="s">
+        <v>46</v>
+      </c>
+      <c r="C144" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D144" s="3">
+        <v>45995.329861111109</v>
+      </c>
+      <c r="E144" s="3">
+        <v>46029.302777777775</v>
+      </c>
+      <c r="F144" s="7">
+        <v>12.421815476888961</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>45</v>
+      </c>
+      <c r="B145" t="s">
+        <v>44</v>
+      </c>
+      <c r="C145" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D145" s="3">
+        <v>45995.366666666669</v>
+      </c>
+      <c r="E145" s="3">
+        <v>46029.366666666669</v>
+      </c>
+      <c r="F145" s="7">
+        <v>29.67314982915925</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>12</v>
+      </c>
+      <c r="B146" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D146" s="3">
+        <v>45995.375</v>
+      </c>
+      <c r="E146" s="3">
+        <v>46029.375</v>
+      </c>
+      <c r="F146" s="7">
+        <v>36.081164675534104</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>43</v>
+      </c>
+      <c r="B147" t="s">
+        <v>42</v>
+      </c>
+      <c r="C147" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D147" s="3"/>
+      <c r="E147" s="3"/>
+      <c r="G147" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>20</v>
+      </c>
+      <c r="B148" t="s">
+        <v>19</v>
+      </c>
+      <c r="C148" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D148" s="3">
+        <v>45995.407638888886</v>
+      </c>
+      <c r="E148" s="3">
+        <v>46029.40902777778</v>
+      </c>
+      <c r="F148" s="7">
+        <v>37.522878465227549</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>22</v>
+      </c>
+      <c r="B149" t="s">
+        <v>21</v>
+      </c>
+      <c r="C149" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D149" s="3">
+        <v>45995.357638888891</v>
+      </c>
+      <c r="E149" s="3">
+        <v>46029.416666666664</v>
+      </c>
+      <c r="F149" s="7">
+        <v>45.75807050916999</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>24</v>
+      </c>
+      <c r="B150" t="s">
+        <v>23</v>
+      </c>
+      <c r="C150" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D150" s="3">
+        <v>45995.417361111111</v>
+      </c>
+      <c r="E150" s="3">
+        <v>46029.432638888888</v>
+      </c>
+      <c r="F150" s="7">
+        <v>14.368279671913369</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>26</v>
+      </c>
+      <c r="B151" t="s">
+        <v>25</v>
+      </c>
+      <c r="C151" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D151" s="3">
+        <v>45995.432638888888</v>
+      </c>
+      <c r="E151" s="3">
+        <v>46029.444444444445</v>
+      </c>
+      <c r="F151" s="7">
+        <v>25.796291930131325</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>41</v>
+      </c>
+      <c r="B152" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D152" s="3">
+        <v>45995.447916666664</v>
+      </c>
+      <c r="E152" s="3">
+        <v>46029.388888888891</v>
+      </c>
+      <c r="F152" s="7">
+        <v>23.710407929803459</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" t="s">
+        <v>36</v>
+      </c>
+      <c r="C153" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D153" s="3">
+        <v>45995.443749999999</v>
+      </c>
+      <c r="E153" s="3">
+        <v>46029.384027777778</v>
+      </c>
+      <c r="F153" s="7">
+        <v>38.342249026535825</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>39</v>
+      </c>
+      <c r="B154" t="s">
+        <v>38</v>
+      </c>
+      <c r="C154" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D154" s="3">
+        <v>45995.435416666667</v>
+      </c>
+      <c r="E154" s="3">
+        <v>46029.379166666666</v>
+      </c>
+      <c r="F154" s="7">
+        <v>36.083131168767828</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>34</v>
+      </c>
+      <c r="B155" t="s">
+        <v>33</v>
+      </c>
+      <c r="C155" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D155" s="3">
+        <v>45995.42083333333</v>
+      </c>
+      <c r="E155" s="3">
+        <v>46029.366666666669</v>
+      </c>
+      <c r="F155" s="7">
+        <v>40.937963138654595</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>32</v>
+      </c>
+      <c r="B156" t="s">
+        <v>31</v>
+      </c>
+      <c r="C156" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D156" s="3">
+        <v>45995.405555555553</v>
+      </c>
+      <c r="E156" s="3">
+        <v>46029.356944444444</v>
+      </c>
+      <c r="F156" s="7">
+        <v>52.840643527195127</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>28</v>
+      </c>
+      <c r="B157" t="s">
+        <v>27</v>
+      </c>
+      <c r="C157" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D157" s="3">
+        <v>45995.394444444442</v>
+      </c>
+      <c r="E157" s="3">
+        <v>46029.348611111112</v>
+      </c>
+      <c r="F157" s="7">
+        <v>29.366357650005266</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>30</v>
+      </c>
+      <c r="B158" t="s">
+        <v>29</v>
+      </c>
+      <c r="C158" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D158" s="3">
+        <v>45995.387499999997</v>
+      </c>
+      <c r="E158" s="3">
+        <v>46029.342361111114</v>
+      </c>
+      <c r="F158" s="7">
+        <v>46.881159384271996</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>18</v>
+      </c>
+      <c r="B159" t="s">
+        <v>17</v>
+      </c>
+      <c r="C159" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D159" s="3">
+        <v>45995.359027777777</v>
+      </c>
+      <c r="E159" s="3">
+        <v>46029.323611111111</v>
+      </c>
+      <c r="F159" s="7">
+        <v>51.259784516387775</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>16</v>
+      </c>
+      <c r="B160" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D160" s="3">
+        <v>45995.371527777781</v>
+      </c>
+      <c r="E160" s="3">
+        <v>46029.333333333336</v>
+      </c>
+      <c r="F160" s="7">
+        <v>23.753657942650701</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>14</v>
+      </c>
+      <c r="B161" t="s">
+        <v>13</v>
+      </c>
+      <c r="C161" s="1">
+        <v>45992</v>
+      </c>
+      <c r="D161" s="3">
+        <v>45995.376388888886</v>
+      </c>
+      <c r="E161" s="3">
+        <v>46029.331250000003</v>
+      </c>
+      <c r="F161" s="7">
+        <v>35.08861127774734</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L141">
     <sortCondition ref="C2:C141"/>
@@ -3684,11 +4085,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68EC4D5B-A80E-3B4D-AB8A-5B05A1610CE9}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3970,7 +4369,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3987,7 +4386,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -4004,7 +4403,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -4021,7 +4420,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -4038,7 +4437,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -4054,6 +4453,126 @@
       <c r="E21" t="s">
         <v>113</v>
       </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H25" s="1"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H26" s="1"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H27" s="1"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H28" s="1"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H29" s="1"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H30" s="1"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H31" s="1"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H32" s="1"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H33" s="1"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H34" s="1"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H35" s="1"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H36" s="1"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H37" s="1"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H38" s="1"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H39" s="1"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H40" s="1"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H41" s="1"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H42" s="1"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H43" s="1"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="8:11" x14ac:dyDescent="0.2">
+      <c r="H44" s="1"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4061,28 +4580,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d2effc7-4260-41d0-876f-94073c520d46">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007862564C6B7D034CBD34C383492C7D58" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="53b9cbb27ea0be9acc74f77401b342f9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d2effc7-4260-41d0-876f-94073c520d46" xmlns:ns3="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1083e288036101acb4c2841bf829040b" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007862564C6B7D034CBD34C383492C7D58" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1206fb82f922ed53daf7d8b34152a514">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d2effc7-4260-41d0-876f-94073c520d46" xmlns:ns3="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1341b299bb0685f98650573ea1918c14" ns2:_="" ns3:_="">
     <xsd:import namespace="0d2effc7-4260-41d0-876f-94073c520d46"/>
     <xsd:import namespace="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9"/>
     <xsd:element name="properties">
@@ -4275,46 +4774,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0d2effc7-4260-41d0-876f-94073c520d46">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89A726DE-ED6C-4B29-9DAB-510946DBBF5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9"/>
-    <ds:schemaRef ds:uri="0d2effc7-4260-41d0-876f-94073c520d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC978141-BE53-4E88-8BCA-2F13FB9F8943}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D234CA42-CCAF-4C6D-881C-C8492E2A638A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFBFDB0A-D714-4D9F-8564-C3A77AF5387E}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FC27487-92EB-4918-ABF3-A8DCA0ADCB9E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0d2effc7-4260-41d0-876f-94073c520d46"/>
-    <ds:schemaRef ds:uri="50fdb4dc-62b1-40b1-81e4-7cb14721f0b9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43174104-FA01-4123-BC4B-623980BB8396}"/>
 </file>
</xml_diff>